<commit_message>
Work on taxa and filters.
</commit_message>
<xml_diff>
--- a/test_data/dwca_matrix_zoobenthos_nat.xlsx
+++ b/test_data/dwca_matrix_zoobenthos_nat.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="687" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="687" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
     <sheet name="field_mapping" sheetId="2" r:id="rId2"/>
     <sheet name="dwc_keys" sheetId="13" r:id="rId3"/>
     <sheet name="dwc_dynamic_fields" sheetId="6" r:id="rId4"/>
-    <sheet name="metadata_mapping" sheetId="7" r:id="rId5"/>
-    <sheet name="filter" sheetId="4" r:id="rId6"/>
+    <sheet name="filter" sheetId="4" r:id="rId5"/>
+    <sheet name="metadata_mapping" sheetId="7" r:id="rId6"/>
     <sheet name="README" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="257">
   <si>
     <t>shark_sample_id_md5</t>
   </si>
@@ -613,12 +613,6 @@
     <t>readme_header_md</t>
   </si>
   <si>
-    <t>included_value</t>
-  </si>
-  <si>
-    <t>excluded_value</t>
-  </si>
-  <si>
     <t>HELCOM-PEG</t>
   </si>
   <si>
@@ -649,36 +643,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>occurrences</t>
-  </si>
-  <si>
-    <t>TEST-samplingEffort-1</t>
-  </si>
-  <si>
-    <t>TEST-samplingEffort-2</t>
-  </si>
-  <si>
-    <t>TEST-samplingProtocol-1</t>
-  </si>
-  <si>
-    <t>TEST-samplingProtocol-2</t>
-  </si>
-  <si>
-    <t>TEST-dynamicProperties-A2</t>
-  </si>
-  <si>
-    <t>TEST-dynamicProperties-B1</t>
-  </si>
-  <si>
-    <t>TEST-dynamicProperties-B2</t>
-  </si>
-  <si>
-    <t>TEST-identificationQualifier-1</t>
-  </si>
-  <si>
-    <t>TEST-identificationQualifier-2</t>
-  </si>
-  <si>
     <t>sample_series</t>
   </si>
   <si>
@@ -779,6 +743,54 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t># eventID</t>
+  </si>
+  <si>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>source_parameter_TODO</t>
+  </si>
+  <si>
+    <t>source_unit_TODO</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>Earlier: measurementRemarks</t>
+  </si>
+  <si>
+    <t>include_value</t>
+  </si>
+  <si>
+    <t>exclude_value</t>
+  </si>
+  <si>
+    <t># SLÄGGÖ</t>
+  </si>
+  <si>
+    <t># N14 FALKENBERG</t>
+  </si>
+  <si>
+    <t># ANHOLT E</t>
+  </si>
+  <si>
+    <t># TOR20</t>
+  </si>
+  <si>
+    <t>delivery_datatype</t>
+  </si>
+  <si>
+    <t>Zooplankton</t>
+  </si>
+  <si>
+    <t># Phytoplankton</t>
+  </si>
+  <si>
+    <t># Zoobenthos</t>
   </si>
 </sst>
 </file>
@@ -822,10 +834,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,18 +1142,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
@@ -1151,7 +1164,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1162,9 +1175,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -1173,7 +1186,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1184,7 +1197,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1195,7 +1208,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1206,7 +1219,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1217,7 +1230,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -1228,7 +1241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -1239,7 +1252,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1263,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1274,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -1272,7 +1285,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -1283,7 +1296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1294,7 +1307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -1305,7 +1318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1316,7 +1329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -1324,7 +1337,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1332,7 +1345,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1340,7 +1353,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1348,7 +1361,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1356,7 +1369,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>104</v>
       </c>
@@ -1364,7 +1377,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1372,7 +1385,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1380,7 +1393,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1396,7 +1409,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -1404,7 +1417,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1412,7 +1425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1420,7 +1433,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -1428,92 +1441,92 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
     </row>
   </sheetData>
@@ -1524,26 +1537,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
@@ -1571,11 +1588,14 @@
       <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -1589,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -1603,7 +1623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -1617,7 +1637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -1631,7 +1651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1645,7 +1665,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -1659,7 +1679,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -1673,7 +1693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>185</v>
       </c>
@@ -1687,10 +1707,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -1704,7 +1724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -1718,7 +1738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -1732,10 +1752,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -1749,7 +1769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -1763,7 +1783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>185</v>
       </c>
@@ -1777,7 +1797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -1791,7 +1811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -1805,7 +1825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -1819,7 +1839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -1833,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -1847,10 +1867,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -1864,7 +1884,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1878,7 +1898,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1892,7 +1912,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -1906,7 +1926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -1920,7 +1940,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>190</v>
       </c>
@@ -1934,21 +1954,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>190</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
-        <v>44</v>
+      <c r="C32" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -1962,7 +1985,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -1979,7 +2002,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -1993,7 +2016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>190</v>
       </c>
@@ -2007,7 +2030,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>190</v>
       </c>
@@ -2021,7 +2044,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>190</v>
       </c>
@@ -2038,7 +2061,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -2052,7 +2075,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>190</v>
       </c>
@@ -2069,7 +2092,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>190</v>
       </c>
@@ -2086,7 +2109,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>190</v>
       </c>
@@ -2103,7 +2126,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>190</v>
       </c>
@@ -2117,7 +2140,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>190</v>
       </c>
@@ -2131,7 +2154,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>190</v>
       </c>
@@ -2145,7 +2168,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>190</v>
       </c>
@@ -2162,7 +2185,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>190</v>
       </c>
@@ -2179,7 +2202,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -2196,7 +2219,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>190</v>
       </c>
@@ -2210,7 +2233,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>190</v>
       </c>
@@ -2224,7 +2247,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>190</v>
       </c>
@@ -2232,7 +2255,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>190</v>
       </c>
@@ -2240,7 +2263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -2248,7 +2271,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -2256,7 +2279,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -2264,7 +2287,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -2272,7 +2295,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -2280,7 +2303,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -2288,7 +2311,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>190</v>
       </c>
@@ -2296,7 +2319,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>190</v>
       </c>
@@ -2304,12 +2327,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -2317,16 +2335,16 @@
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E66" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F66" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>185</v>
       </c>
@@ -2334,13 +2352,13 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I68" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>185</v>
       </c>
@@ -2354,7 +2372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>185</v>
       </c>
@@ -2368,7 +2386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>185</v>
       </c>
@@ -2382,7 +2400,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>64</v>
       </c>
@@ -2396,14 +2414,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="68" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2415,21 +2433,21 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="15" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" customWidth="1"/>
+    <col min="12" max="15" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2570,22 +2588,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="6" width="24.26953125" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -2599,16 +2620,16 @@
         <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>193</v>
+        <v>244</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2616,13 +2637,13 @@
         <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2630,113 +2651,99 @@
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="D4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>212</v>
-      </c>
-      <c r="G8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="D9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>247</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
-      </c>
-      <c r="G13" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="D13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>83</v>
@@ -2744,288 +2751,256 @@
       <c r="C14" t="s">
         <v>214</v>
       </c>
-      <c r="G14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="D16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
         <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="D19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>209</v>
       </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D22" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>209</v>
-      </c>
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>227</v>
-      </c>
       <c r="D23" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>209</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D25" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>209</v>
-      </c>
-      <c r="B26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" t="s">
-        <v>230</v>
-      </c>
-      <c r="D26" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>231</v>
-      </c>
-      <c r="D27" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>209</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>232</v>
-      </c>
-      <c r="D28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>209</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>233</v>
-      </c>
-      <c r="D29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>209</v>
-      </c>
-      <c r="B31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" t="s">
-        <v>217</v>
-      </c>
-      <c r="G31" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>209</v>
-      </c>
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" t="s">
-        <v>218</v>
-      </c>
-      <c r="G32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" t="s">
-        <v>221</v>
-      </c>
-      <c r="D34" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" t="s">
-        <v>222</v>
-      </c>
-      <c r="D35" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" t="s">
-        <v>223</v>
-      </c>
-      <c r="D36" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3050,13 +3025,13 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3064,13 +3039,13 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
         <v>203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3078,53 +3053,15 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3132,13 +3069,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="210.140625" customWidth="1"/>
+    <col min="1" max="1" width="87.81640625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Metadata fix. Added test data.
</commit_message>
<xml_diff>
--- a/test_data/dwca_matrix_zoobenthos_nat.xlsx
+++ b/test_data/dwca_matrix_zoobenthos_nat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="687" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="687"/>
   </bookViews>
   <sheets>
     <sheet name="dwc_columns" sheetId="12" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="265">
   <si>
     <t>shark_sample_id_md5</t>
   </si>
@@ -298,9 +298,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>eventID</t>
-  </si>
-  <si>
     <t>parentEventID</t>
   </si>
   <si>
@@ -812,6 +809,12 @@
   </si>
   <si>
     <t>dataset_file_name</t>
+  </si>
+  <si>
+    <t>MethodDocumentation</t>
+  </si>
+  <si>
+    <t>method_documentation</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1176,13 +1179,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1198,35 +1201,35 @@
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1234,10 +1237,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1245,21 +1248,21 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1270,7 +1273,7 @@
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1281,7 +1284,7 @@
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1292,26 +1295,26 @@
         <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1322,7 +1325,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
@@ -1330,10 +1333,10 @@
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>42</v>
@@ -1341,10 +1344,10 @@
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -1352,18 +1355,18 @@
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1371,7 +1374,7 @@
         <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1379,7 +1382,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1387,15 +1390,15 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1403,7 +1406,7 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1411,7 +1414,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1419,7 +1422,7 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1427,12 +1430,12 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
         <v>79</v>
@@ -1451,12 +1454,12 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
         <v>82</v>
@@ -1484,12 +1487,12 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
@@ -1499,27 +1502,27 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
@@ -1539,7 +1542,7 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
@@ -1563,8 +1566,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,28 +1584,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1610,7 +1613,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -1638,7 +1641,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
@@ -1652,7 +1655,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -1666,7 +1669,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
@@ -1683,7 +1686,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
@@ -1700,7 +1703,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
@@ -1714,7 +1717,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
@@ -1731,7 +1734,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -1743,12 +1746,12 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -1760,12 +1763,12 @@
         <v>18</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
@@ -1777,7 +1780,7 @@
         <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1785,35 +1788,35 @@
     </row>
     <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>62</v>
@@ -1822,12 +1825,12 @@
         <v>32</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>63</v>
@@ -1836,35 +1839,35 @@
         <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1872,275 +1875,275 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B32" t="s">
         <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
         <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B35" t="s">
         <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B36" t="s">
         <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
         <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B39" t="s">
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G41" t="s">
         <v>76</v>
@@ -2148,7 +2151,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B42" t="s">
         <v>62</v>
@@ -2162,7 +2165,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B43" t="s">
         <v>62</v>
@@ -2176,7 +2179,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B44" t="s">
         <v>62</v>
@@ -2185,7 +2188,7 @@
         <v>46</v>
       </c>
       <c r="F44" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G44" t="s">
         <v>77</v>
@@ -2194,7 +2197,7 @@
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B46" t="s">
         <v>63</v>
@@ -2208,7 +2211,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B47" t="s">
         <v>63</v>
@@ -2222,7 +2225,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B48" t="s">
         <v>63</v>
@@ -2236,7 +2239,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B49" t="s">
         <v>63</v>
@@ -2250,7 +2253,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
         <v>63</v>
@@ -2264,7 +2267,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B51" t="s">
         <v>63</v>
@@ -2276,12 +2279,12 @@
         <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
@@ -2295,7 +2298,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B53" t="s">
         <v>63</v>
@@ -2369,24 +2372,24 @@
     <row r="59" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>64</v>
@@ -2400,7 +2403,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>64</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>64</v>
@@ -2428,7 +2431,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>64</v>
@@ -2443,7 +2446,7 @@
     <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2456,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2473,25 +2476,26 @@
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="16.81640625" customWidth="1"/>
-    <col min="12" max="15" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6328125" customWidth="1"/>
+    <col min="13" max="15" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>87</v>
@@ -2529,7 +2533,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -2552,7 +2556,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -2607,10 +2611,13 @@
       <c r="K7" t="s">
         <v>66</v>
       </c>
+      <c r="L7" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>62</v>
@@ -2625,7 +2632,7 @@
     <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>63</v>
@@ -2639,7 +2646,7 @@
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2661,10 +2668,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2678,10 +2685,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>85</v>
@@ -2690,7 +2697,7 @@
         <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>75</v>
@@ -2698,7 +2705,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -2707,7 +2714,7 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -2715,7 +2722,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -2724,15 +2731,15 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" t="s">
         <v>229</v>
-      </c>
-      <c r="E4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -2741,15 +2748,15 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
@@ -2758,32 +2765,32 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9" t="s">
-        <v>224</v>
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
@@ -2792,32 +2799,32 @@
         <v>82</v>
       </c>
       <c r="D10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" t="s">
         <v>223</v>
       </c>
-      <c r="E10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>254</v>
-      </c>
-      <c r="E12" t="s">
-        <v>202</v>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>63</v>
@@ -2826,15 +2833,15 @@
         <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -2843,27 +2850,27 @@
         <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2877,10 +2884,10 @@
         <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2894,10 +2901,10 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E18" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2911,7 +2918,7 @@
         <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E19" t="s">
         <v>220</v>
@@ -2928,7 +2935,7 @@
         <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
         <v>219</v>
@@ -2945,7 +2952,7 @@
         <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E21" t="s">
         <v>218</v>
@@ -2962,7 +2969,7 @@
         <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E22" t="s">
         <v>217</v>
@@ -2979,7 +2986,7 @@
         <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E23" t="s">
         <v>216</v>
@@ -2996,7 +3003,7 @@
         <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E24" t="s">
         <v>215</v>
@@ -3013,10 +3020,27 @@
         <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E25" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3040,37 +3064,37 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
         <v>241</v>
-      </c>
-      <c r="B3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -3079,7 +3103,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -3087,7 +3111,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -3095,7 +3119,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -3103,7 +3127,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -3111,10 +3135,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -3122,7 +3146,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -3130,7 +3154,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3154,19 +3178,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3174,13 +3198,13 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,13 +3212,13 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3202,10 +3226,10 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" t="s">
         <v>200</v>
-      </c>
-      <c r="E7" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>